<commit_message>
Adding control signals to decoder. Not yet tested.
</commit_message>
<xml_diff>
--- a/new_code/instruction breakdown.xlsx
+++ b/new_code/instruction breakdown.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Control signals" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Opcode</t>
   </si>
@@ -111,9 +111,6 @@
     <t>All 0s</t>
   </si>
   <si>
-    <t>&lt;-- rt</t>
-  </si>
-  <si>
     <t>ADDIU</t>
   </si>
   <si>
@@ -127,6 +124,111 @@
   </si>
   <si>
     <t>ORI</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>Contorl Signal</t>
+  </si>
+  <si>
+    <t>Signed/unsigned</t>
+  </si>
+  <si>
+    <t>Sub/add</t>
+  </si>
+  <si>
+    <t>Shift direction</t>
+  </si>
+  <si>
+    <t>Shift sign</t>
+  </si>
+  <si>
+    <t>Num Bits</t>
+  </si>
+  <si>
+    <t>Branch insn</t>
+  </si>
+  <si>
+    <t>Immediate insn</t>
+  </si>
+  <si>
+    <t>sign extended or not</t>
+  </si>
+  <si>
+    <t>Signed comparison</t>
+  </si>
+  <si>
+    <t>Zero</t>
+  </si>
+  <si>
+    <t>imme_control</t>
+  </si>
+  <si>
+    <t>sign_extended_control</t>
+  </si>
+  <si>
+    <t>alu_signed_ctl</t>
+  </si>
+  <si>
+    <t>alu_op_ctl</t>
+  </si>
+  <si>
+    <t>shift_dir_ctl</t>
+  </si>
+  <si>
+    <t>shift_sign_ctl</t>
+  </si>
+  <si>
+    <t>branch_ctl</t>
+  </si>
+  <si>
+    <t>logical_op_ctl</t>
+  </si>
+  <si>
+    <t>slt_ctl</t>
+  </si>
+  <si>
+    <t>shift_amt_ctl</t>
+  </si>
+  <si>
+    <t>Output Mux</t>
+  </si>
+  <si>
+    <t>ALU</t>
+  </si>
+  <si>
+    <t>jump</t>
+  </si>
+  <si>
+    <t>shifter</t>
+  </si>
+  <si>
+    <t>logical</t>
+  </si>
+  <si>
+    <t>branch</t>
+  </si>
+  <si>
+    <t>not used</t>
+  </si>
+  <si>
+    <t>bit index</t>
+  </si>
+  <si>
+    <t>8..6</t>
+  </si>
+  <si>
+    <t>10..9</t>
+  </si>
+  <si>
+    <t>16..12</t>
+  </si>
+  <si>
+    <t>19..17</t>
+  </si>
+  <si>
+    <t>Bits</t>
   </si>
 </sst>
 </file>
@@ -192,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -204,12 +306,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -500,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -509,6 +621,7 @@
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -532,6 +645,9 @@
       <c r="C2" s="1">
         <v>0</v>
       </c>
+      <c r="D2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
@@ -675,9 +791,6 @@
       <c r="C15" s="10">
         <v>0</v>
       </c>
-      <c r="D15" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="6" t="s">
@@ -689,9 +802,6 @@
       <c r="C16" s="10">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
@@ -743,7 +853,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>1001</v>
@@ -756,18 +866,24 @@
       <c r="B24" s="1">
         <v>1010</v>
       </c>
+      <c r="D24" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="1">
         <v>1101</v>
       </c>
+      <c r="D25" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="1">
         <v>1111</v>
@@ -802,7 +918,7 @@
         <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -810,7 +926,7 @@
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -824,13 +940,270 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="B9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" s="12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="C20" s="12"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" s="13">
+        <v>3</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
- Added JAL and JR support to decode stage (still needs to be added to execute stage) - Adding memory stage (mem2.vhd) - Adding writeback stage, still needs to be implemented - Connected everything up in tb.vhd Note: Since writeback is not yet implemented, running the modified tb causes a fatal error during simulation due to negative array index in mem2. Comment out mem2 read/write logic to make it work.
</commit_message>
<xml_diff>
--- a/new_code/instruction breakdown.xlsx
+++ b/new_code/instruction breakdown.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>Opcode</t>
   </si>
@@ -138,24 +138,9 @@
     <t>Sub/add</t>
   </si>
   <si>
-    <t>Shift direction</t>
-  </si>
-  <si>
-    <t>Shift sign</t>
-  </si>
-  <si>
     <t>Num Bits</t>
   </si>
   <si>
-    <t>Branch insn</t>
-  </si>
-  <si>
-    <t>Immediate insn</t>
-  </si>
-  <si>
-    <t>sign extended or not</t>
-  </si>
-  <si>
     <t>Signed comparison</t>
   </si>
   <si>
@@ -229,6 +214,36 @@
   </si>
   <si>
     <t>Bits</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>mem_we</t>
+  </si>
+  <si>
+    <t>dest_reg</t>
+  </si>
+  <si>
+    <t>25..21</t>
+  </si>
+  <si>
+    <t>wb_select</t>
+  </si>
+  <si>
+    <t>0=exec, 1=mem</t>
+  </si>
+  <si>
+    <t>wb_disable</t>
+  </si>
+  <si>
+    <t>0=do wb,1=no wb</t>
+  </si>
+  <si>
+    <t>JR</t>
+  </si>
+  <si>
+    <t>JAL</t>
   </si>
 </sst>
 </file>
@@ -306,11 +321,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -610,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -624,7 +641,7 @@
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -635,7 +652,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -649,7 +666,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -660,7 +677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
@@ -671,7 +688,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -682,7 +699,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -692,8 +709,11 @@
       <c r="C6" s="1">
         <v>100001</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -704,7 +724,7 @@
         <v>100010</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -715,7 +735,7 @@
         <v>100011</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
@@ -726,7 +746,7 @@
         <v>100100</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -737,7 +757,7 @@
         <v>100101</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -748,7 +768,7 @@
         <v>100110</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -759,7 +779,7 @@
         <v>100111</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
@@ -770,7 +790,7 @@
         <v>101010</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
         <v>9</v>
       </c>
@@ -781,7 +801,7 @@
         <v>101011</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" s="8" t="s">
         <v>27</v>
       </c>
@@ -792,7 +812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
         <v>24</v>
       </c>
@@ -803,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -811,7 +831,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -819,7 +839,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -827,7 +847,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -835,7 +855,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -843,7 +863,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -851,15 +871,18 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>1001</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -867,10 +890,10 @@
         <v>1010</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -878,10 +901,10 @@
         <v>1101</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -889,44 +912,59 @@
         <v>1111</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="1">
         <v>100011</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="1">
         <v>101011</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>19</v>
       </c>
       <c r="D30" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>20</v>
       </c>
       <c r="D31" t="s">
         <v>32</v>
+      </c>
+      <c r="E31" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -940,16 +978,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1">
@@ -957,7 +996,7 @@
         <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -977,53 +1016,69 @@
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="11"/>
+      <c r="B4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="6">
-        <v>1</v>
-      </c>
-      <c r="C5" s="11"/>
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>1</v>
+      </c>
+      <c r="C7" s="11">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8" s="11">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="B9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>65</v>
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="11">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1033,8 +1088,8 @@
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="12">
-        <v>0</v>
+      <c r="C10" s="11">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1042,10 +1097,10 @@
         <v>49</v>
       </c>
       <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="12">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1053,13 +1108,10 @@
         <v>50</v>
       </c>
       <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="12">
         <v>2</v>
       </c>
-      <c r="D12" t="s">
-        <v>64</v>
+      <c r="C12" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1069,8 +1121,8 @@
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="12">
-        <v>3</v>
+      <c r="C13" s="11">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1078,130 +1130,150 @@
         <v>52</v>
       </c>
       <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="12">
+        <v>5</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="C15" s="11"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="12">
+        <v>3</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17" s="13"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" s="13"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" s="13"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" s="13"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" s="12">
+      <c r="C21" s="13"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+      <c r="C22" s="13"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>55</v>
       </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" s="12" t="s">
+      <c r="B23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19">
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27">
         <v>5</v>
       </c>
-      <c r="C19" s="12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="C20" s="12"/>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="13">
-        <v>3</v>
-      </c>
-      <c r="C21" s="12" t="s">
+      <c r="C27" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
-        <v>60</v>
-      </c>
-      <c r="B27">
-        <v>6</v>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>26</v>
+      </c>
+      <c r="D28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C17:C22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>